<commit_message>
Nearly done with the restructuring and renormalising of python scripts.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data_new_order/data/cleaned_data_for_overlay.xlsx
+++ b/DATA/collate_cultivar_data_new_order/data/cleaned_data_for_overlay.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="2">
   <si>
-    <t>kcp</t>
+    <t>y_scatter</t>
   </si>
   <si>
-    <t>datetimeStamp</t>
+    <t>datetime_stamp</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Finished the bash pipelines.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data_new_order/data/cleaned_data_for_overlay.xlsx
+++ b/DATA/collate_cultivar_data_new_order/data/cleaned_data_for_overlay.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -421,194 +421,418 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>43155</v>
+        <v>43145</v>
       </c>
       <c r="B4">
-        <v>0.3726708</v>
+        <v>0.2583732</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>43161</v>
+        <v>43149</v>
       </c>
       <c r="B5">
-        <v>0.6275229</v>
+        <v>0.3292929</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>43173</v>
+        <v>43155</v>
       </c>
       <c r="B6">
-        <v>0.5809935000000001</v>
+        <v>0.3726708</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>43185</v>
+        <v>43161</v>
       </c>
       <c r="B7">
-        <v>0.372591</v>
+        <v>0.6275229</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>43197</v>
+        <v>43173</v>
       </c>
       <c r="B8">
-        <v>0.4118896</v>
+        <v>0.5809935000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>43202</v>
+        <v>43174</v>
       </c>
       <c r="B9">
-        <v>0.3298969</v>
+        <v>0.3484848</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>43215</v>
+        <v>43175</v>
       </c>
       <c r="B10">
-        <v>0.3725</v>
+        <v>0.3363844</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>43243</v>
+        <v>43176</v>
       </c>
       <c r="B11">
-        <v>0.2008547</v>
+        <v>0.3449692</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>43244</v>
+        <v>43183</v>
       </c>
       <c r="B12">
-        <v>0.2469636</v>
+        <v>0.3318486</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>42924</v>
+        <v>43184</v>
       </c>
       <c r="B13">
-        <v>0.0790698</v>
+        <v>0.2696391</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>42998</v>
+        <v>43185</v>
       </c>
       <c r="B14">
-        <v>0.0828829</v>
+        <v>0.372591</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>43004</v>
+        <v>43186</v>
       </c>
       <c r="B15">
-        <v>0.09905659999999999</v>
+        <v>0.3031088</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>43006</v>
+        <v>43191</v>
       </c>
       <c r="B16">
-        <v>0.07805910000000001</v>
+        <v>0.2094118</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>43009</v>
+        <v>43197</v>
       </c>
       <c r="B17">
-        <v>0.1840278</v>
+        <v>0.4118896</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>43019</v>
+        <v>43201</v>
       </c>
       <c r="B18">
-        <v>0.1901408</v>
+        <v>0.2534819</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>43053</v>
+        <v>43202</v>
       </c>
       <c r="B19">
-        <v>0.2363014</v>
+        <v>0.3298969</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>43064</v>
+        <v>43204</v>
       </c>
       <c r="B20">
-        <v>0.2549669</v>
+        <v>0.2301887</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>43072</v>
+        <v>43215</v>
       </c>
       <c r="B21">
-        <v>0.5276381999999999</v>
+        <v>0.3725</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>43172</v>
+        <v>43218</v>
       </c>
       <c r="B22">
-        <v>0.5953608</v>
+        <v>0.5684932</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>43177</v>
+        <v>43223</v>
       </c>
       <c r="B23">
-        <v>0.5670103</v>
+        <v>0.2661064</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>43183</v>
+        <v>43243</v>
       </c>
       <c r="B24">
-        <v>0.4403292</v>
+        <v>0.2008547</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>43238</v>
+        <v>43244</v>
       </c>
       <c r="B25">
-        <v>0.2558824</v>
+        <v>0.2469636</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>43176</v>
+        <v>43248</v>
       </c>
       <c r="B26">
-        <v>0.5494505</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
+        <v>43252</v>
+      </c>
+      <c r="B27">
+        <v>0.0662021</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2">
+        <v>42922</v>
+      </c>
+      <c r="B28">
+        <v>0.1399417</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2">
+        <v>42924</v>
+      </c>
+      <c r="B29">
+        <v>0.0790698</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2">
+        <v>42998</v>
+      </c>
+      <c r="B30">
+        <v>0.0828829</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2">
+        <v>43004</v>
+      </c>
+      <c r="B31">
+        <v>0.09905659999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
+        <v>43006</v>
+      </c>
+      <c r="B32">
+        <v>0.07805910000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
+        <v>43009</v>
+      </c>
+      <c r="B33">
+        <v>0.1840278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2">
+        <v>43019</v>
+      </c>
+      <c r="B34">
+        <v>0.1901408</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2">
+        <v>43020</v>
+      </c>
+      <c r="B35">
+        <v>0.0886364</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2">
+        <v>43053</v>
+      </c>
+      <c r="B36">
+        <v>0.2363014</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2">
+        <v>43059</v>
+      </c>
+      <c r="B37">
+        <v>0.3988604</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2">
+        <v>43063</v>
+      </c>
+      <c r="B38">
+        <v>0.4010417</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2">
+        <v>43064</v>
+      </c>
+      <c r="B39">
+        <v>0.2549669</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2">
+        <v>43065</v>
+      </c>
+      <c r="B40">
+        <v>0.1949405</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2">
+        <v>43066</v>
+      </c>
+      <c r="B41">
+        <v>0.188251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2">
+        <v>43072</v>
+      </c>
+      <c r="B42">
+        <v>0.5276381999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2">
+        <v>43073</v>
+      </c>
+      <c r="B43">
+        <v>0.2886957</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2">
+        <v>43164</v>
+      </c>
+      <c r="B44">
+        <v>0.6550459</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2">
+        <v>43172</v>
+      </c>
+      <c r="B45">
+        <v>0.5953608</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2">
+        <v>43173</v>
+      </c>
+      <c r="B46">
+        <v>0.327381</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2">
+        <v>43177</v>
+      </c>
+      <c r="B47">
+        <v>0.5670103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2">
+        <v>43178</v>
+      </c>
+      <c r="B48">
+        <v>0.2719101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2">
+        <v>43183</v>
+      </c>
+      <c r="B49">
+        <v>0.4403292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2">
+        <v>43237</v>
+      </c>
+      <c r="B50">
+        <v>0.2754491</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2">
+        <v>43238</v>
+      </c>
+      <c r="B51">
+        <v>0.2558824</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2">
+        <v>42971</v>
+      </c>
+      <c r="B52">
+        <v>0.1628788</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2">
+        <v>43176</v>
+      </c>
+      <c r="B53">
+        <v>0.5494505</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2">
         <v>43182</v>
       </c>
-      <c r="B27">
+      <c r="B54">
         <v>0.5160681</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2">
+        <v>43184</v>
+      </c>
+      <c r="B55">
+        <v>0.3086053</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +842,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -690,137 +914,209 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>42954</v>
+        <v>43145</v>
       </c>
       <c r="B9">
-        <v>0.1157025</v>
+        <v>0.430622</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>42994</v>
+        <v>42954</v>
       </c>
       <c r="B10">
-        <v>0.1049563</v>
+        <v>0.1157025</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>43004</v>
+        <v>42955</v>
       </c>
       <c r="B11">
-        <v>0.0943396</v>
+        <v>0.0695971</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>43008</v>
+        <v>42992</v>
       </c>
       <c r="B12">
-        <v>0.1163311</v>
+        <v>0.0506757</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>43013</v>
+        <v>42994</v>
       </c>
       <c r="B13">
-        <v>0.1122807</v>
+        <v>0.1049563</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>43019</v>
+        <v>43004</v>
       </c>
       <c r="B14">
-        <v>0.1267606</v>
+        <v>0.0943396</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>43037</v>
+        <v>43006</v>
       </c>
       <c r="B15">
-        <v>0.1193353</v>
+        <v>0.1329114</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>43038</v>
+        <v>43008</v>
       </c>
       <c r="B16">
-        <v>0.1136045</v>
+        <v>0.1163311</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>43046</v>
+        <v>43013</v>
       </c>
       <c r="B17">
-        <v>0.343879</v>
+        <v>0.1122807</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>43050</v>
+        <v>43018</v>
       </c>
       <c r="B18">
-        <v>0.3513011</v>
+        <v>0.2144578</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>43079</v>
+        <v>43019</v>
       </c>
       <c r="B19">
-        <v>0.5490196000000001</v>
+        <v>0.1267606</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>43106</v>
+        <v>43021</v>
       </c>
       <c r="B20">
-        <v>0.4017857</v>
+        <v>0.09003220000000001</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>43111</v>
+        <v>43035</v>
       </c>
       <c r="B21">
-        <v>0.4267442</v>
+        <v>0.1031308</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>43120</v>
+        <v>43037</v>
       </c>
       <c r="B22">
-        <v>0.5944584000000001</v>
+        <v>0.1193353</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>43150</v>
+        <v>43038</v>
       </c>
       <c r="B23">
-        <v>0.4237288</v>
+        <v>0.1136045</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>42935</v>
+        <v>43046</v>
       </c>
       <c r="B24">
-        <v>0.1029186</v>
+        <v>0.343879</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
+        <v>43050</v>
+      </c>
+      <c r="B25">
+        <v>0.3513011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2">
+        <v>43079</v>
+      </c>
+      <c r="B26">
+        <v>0.5490196000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2">
+        <v>43106</v>
+      </c>
+      <c r="B27">
+        <v>0.4017857</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2">
+        <v>43111</v>
+      </c>
+      <c r="B28">
+        <v>0.4267442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2">
+        <v>43120</v>
+      </c>
+      <c r="B29">
+        <v>0.5944584000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2">
+        <v>43150</v>
+      </c>
+      <c r="B30">
+        <v>0.4237288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2">
+        <v>42935</v>
+      </c>
+      <c r="B31">
+        <v>0.1029186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
+        <v>43071</v>
+      </c>
+      <c r="B32">
+        <v>0.7166667</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
+        <v>43115</v>
+      </c>
+      <c r="B33">
+        <v>0.6528777</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2">
         <v>43127</v>
       </c>
-      <c r="B25">
+      <c r="B34">
         <v>0.5355932</v>
       </c>
     </row>
@@ -831,7 +1127,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -855,330 +1151,546 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>43116</v>
+        <v>43107</v>
       </c>
       <c r="B3">
-        <v>0.5072464</v>
+        <v>0.6779412</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>43147</v>
+        <v>43116</v>
       </c>
       <c r="B4">
-        <v>0.4797794</v>
+        <v>0.5072464</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>43148</v>
+        <v>43121</v>
       </c>
       <c r="B5">
-        <v>0.4540902</v>
+        <v>0.3323944</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>43155</v>
+        <v>43147</v>
       </c>
       <c r="B6">
-        <v>0.6169772</v>
+        <v>0.4797794</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>43159</v>
+        <v>43148</v>
       </c>
       <c r="B7">
-        <v>0.4646782</v>
+        <v>0.4540902</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>43164</v>
+        <v>43155</v>
       </c>
       <c r="B8">
-        <v>0.5961071</v>
+        <v>0.6169772</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>43172</v>
+        <v>43159</v>
       </c>
       <c r="B9">
-        <v>0.5270506</v>
+        <v>0.4646782</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>43204</v>
+        <v>43160</v>
       </c>
       <c r="B10">
-        <v>0.5169811</v>
+        <v>0.3193431</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>43222</v>
+        <v>43164</v>
       </c>
       <c r="B11">
-        <v>0.2412587</v>
+        <v>0.5961071</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>43239</v>
+        <v>43169</v>
       </c>
       <c r="B12">
-        <v>0.2258065</v>
+        <v>0.2711864</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>43247</v>
+        <v>43172</v>
       </c>
       <c r="B13">
-        <v>0.1504065</v>
+        <v>0.5270506</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>43248</v>
+        <v>43183</v>
       </c>
       <c r="B14">
-        <v>0.25</v>
+        <v>0.2694878</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>42923</v>
+        <v>43201</v>
       </c>
       <c r="B15">
-        <v>0.111465</v>
+        <v>0.264624</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>42987</v>
+        <v>43202</v>
       </c>
       <c r="B16">
-        <v>0.1233596</v>
+        <v>0.2749141</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>42993</v>
+        <v>43204</v>
       </c>
       <c r="B17">
-        <v>0.0898876</v>
+        <v>0.5169811</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>42995</v>
+        <v>43213</v>
       </c>
       <c r="B18">
-        <v>0.1072261</v>
+        <v>0.540305</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>43020</v>
+        <v>43222</v>
       </c>
       <c r="B19">
-        <v>0.1840909</v>
+        <v>0.2412587</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>43078</v>
+        <v>43239</v>
       </c>
       <c r="B20">
-        <v>0.5905849</v>
+        <v>0.2258065</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>43081</v>
+        <v>43247</v>
       </c>
       <c r="B21">
-        <v>0.4270073</v>
+        <v>0.1504065</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>43091</v>
+        <v>43248</v>
       </c>
       <c r="B22">
-        <v>0.5403846</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>43104</v>
+        <v>42923</v>
       </c>
       <c r="B23">
-        <v>0.5102564000000001</v>
+        <v>0.111465</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>43115</v>
+        <v>42947</v>
       </c>
       <c r="B24">
-        <v>0.6269231</v>
+        <v>0.0518359</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>43124</v>
+        <v>42954</v>
       </c>
       <c r="B25">
-        <v>0.3915663</v>
+        <v>0.0619835</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>43126</v>
+        <v>42987</v>
       </c>
       <c r="B26">
-        <v>0.4245723</v>
+        <v>0.1233596</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>43131</v>
+        <v>42993</v>
       </c>
       <c r="B27">
-        <v>0.423913</v>
+        <v>0.0898876</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>43138</v>
+        <v>42995</v>
       </c>
       <c r="B28">
-        <v>0.3982169</v>
+        <v>0.1072261</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>43145</v>
+        <v>43002</v>
       </c>
       <c r="B29">
-        <v>0.374031</v>
+        <v>0.1352041</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>43155</v>
+        <v>43008</v>
       </c>
       <c r="B30">
-        <v>0.3855799</v>
+        <v>0.1431767</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>43163</v>
+        <v>43020</v>
       </c>
       <c r="B31">
-        <v>0.3631285</v>
+        <v>0.1840909</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>43171</v>
+        <v>43078</v>
       </c>
       <c r="B32">
-        <v>0.5</v>
+        <v>0.5905849</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>43172</v>
+        <v>43081</v>
       </c>
       <c r="B33">
-        <v>0.4123711</v>
+        <v>0.4270073</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>43176</v>
+        <v>43089</v>
       </c>
       <c r="B34">
-        <v>0.592668</v>
+        <v>0.3305085</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>43192</v>
+        <v>43091</v>
       </c>
       <c r="B35">
-        <v>0.3431085</v>
+        <v>0.5403846</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>43206</v>
+        <v>43104</v>
       </c>
       <c r="B36">
-        <v>0.4387528</v>
+        <v>0.5102564000000001</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>43207</v>
+        <v>43115</v>
       </c>
       <c r="B37">
-        <v>0.3364486</v>
+        <v>0.6269231</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>42938</v>
+        <v>43124</v>
       </c>
       <c r="B38">
-        <v>0.1077694</v>
+        <v>0.3915663</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>42939</v>
+        <v>43126</v>
       </c>
       <c r="B39">
-        <v>0.1149733</v>
+        <v>0.4245723</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>42942</v>
+        <v>43127</v>
       </c>
       <c r="B40">
-        <v>0.1221374</v>
+        <v>0.2616984</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>43013</v>
+        <v>43131</v>
       </c>
       <c r="B41">
-        <v>0.1679389</v>
+        <v>0.423913</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>43014</v>
+        <v>43138</v>
       </c>
       <c r="B42">
-        <v>0.1236364</v>
+        <v>0.3982169</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
+        <v>43142</v>
+      </c>
+      <c r="B43">
+        <v>0.3075862</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2">
+        <v>43145</v>
+      </c>
+      <c r="B44">
+        <v>0.374031</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2">
+        <v>43148</v>
+      </c>
+      <c r="B45">
+        <v>0.2956204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2">
+        <v>43152</v>
+      </c>
+      <c r="B46">
+        <v>0.3078125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2">
+        <v>43155</v>
+      </c>
+      <c r="B47">
+        <v>0.3855799</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2">
+        <v>43163</v>
+      </c>
+      <c r="B48">
+        <v>0.3631285</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2">
+        <v>43171</v>
+      </c>
+      <c r="B49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2">
+        <v>43172</v>
+      </c>
+      <c r="B50">
+        <v>0.4123711</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2">
+        <v>43173</v>
+      </c>
+      <c r="B51">
+        <v>0.264881</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2">
+        <v>43176</v>
+      </c>
+      <c r="B52">
+        <v>0.592668</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2">
+        <v>43177</v>
+      </c>
+      <c r="B53">
+        <v>0.2927835</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2">
+        <v>43192</v>
+      </c>
+      <c r="B54">
+        <v>0.3431085</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2">
+        <v>43195</v>
+      </c>
+      <c r="B55">
+        <v>0.2135678</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2">
+        <v>43206</v>
+      </c>
+      <c r="B56">
+        <v>0.4387528</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2">
+        <v>43207</v>
+      </c>
+      <c r="B57">
+        <v>0.3364486</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2">
+        <v>43209</v>
+      </c>
+      <c r="B58">
+        <v>0.2171429</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="2">
+        <v>42927</v>
+      </c>
+      <c r="B59">
+        <v>0.1407942</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="2">
+        <v>42938</v>
+      </c>
+      <c r="B60">
+        <v>0.1077694</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2">
+        <v>42939</v>
+      </c>
+      <c r="B61">
+        <v>0.1149733</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="2">
+        <v>42942</v>
+      </c>
+      <c r="B62">
+        <v>0.1221374</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="2">
+        <v>43011</v>
+      </c>
+      <c r="B63">
+        <v>0.2232824</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2">
+        <v>43012</v>
+      </c>
+      <c r="B64">
+        <v>0.2140078</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2">
+        <v>43013</v>
+      </c>
+      <c r="B65">
+        <v>0.1679389</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2">
+        <v>43014</v>
+      </c>
+      <c r="B66">
+        <v>0.1236364</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2">
         <v>43015</v>
       </c>
-      <c r="B43">
+      <c r="B67">
         <v>0.1941075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2">
+        <v>43023</v>
+      </c>
+      <c r="B68">
+        <v>0.2152174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2">
+        <v>43127</v>
+      </c>
+      <c r="B69">
+        <v>0.6898305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2">
+        <v>43138</v>
+      </c>
+      <c r="B70">
+        <v>0.6666666999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1700,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1204,634 +1716,1090 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>43114</v>
+        <v>43107</v>
       </c>
       <c r="B2">
-        <v>0.6212361</v>
+        <v>0.2897059</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>43120</v>
+        <v>43114</v>
       </c>
       <c r="B3">
-        <v>0.5660036000000001</v>
+        <v>0.6212361</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>43128</v>
+        <v>43120</v>
       </c>
       <c r="B4">
-        <v>0.4456522</v>
+        <v>0.5660036000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>43151</v>
+        <v>43128</v>
       </c>
       <c r="B5">
-        <v>0.585736</v>
+        <v>0.4456522</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>43168</v>
+        <v>43148</v>
       </c>
       <c r="B6">
-        <v>0.5582734</v>
+        <v>0.2704508</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>43216</v>
+        <v>43150</v>
       </c>
       <c r="B7">
-        <v>0.3418079</v>
+        <v>0.6924101</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>43233</v>
+        <v>43151</v>
       </c>
       <c r="B8">
-        <v>0.2086168</v>
+        <v>0.585736</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>43234</v>
+        <v>43157</v>
       </c>
       <c r="B9">
-        <v>0.1458333</v>
+        <v>0.6780924</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>42922</v>
+        <v>43158</v>
       </c>
       <c r="B10">
-        <v>0.1253644</v>
+        <v>0.3363636</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>42923</v>
+        <v>43165</v>
       </c>
       <c r="B11">
-        <v>0.1050955</v>
+        <v>0.3452381</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>42924</v>
+        <v>43168</v>
       </c>
       <c r="B12">
-        <v>0.1209302</v>
+        <v>0.5582734</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>42940</v>
+        <v>43172</v>
       </c>
       <c r="B13">
-        <v>0.0988024</v>
+        <v>0.3228621</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>42946</v>
+        <v>43188</v>
       </c>
       <c r="B14">
-        <v>0.1030303</v>
+        <v>0.6512605</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>42947</v>
+        <v>43200</v>
       </c>
       <c r="B15">
-        <v>0.1187905</v>
+        <v>0.2057143</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>42950</v>
+        <v>43213</v>
       </c>
       <c r="B16">
-        <v>0.1437908</v>
+        <v>0.2135076</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>42951</v>
+        <v>43216</v>
       </c>
       <c r="B17">
-        <v>0.1384615</v>
+        <v>0.3418079</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>42952</v>
+        <v>43233</v>
       </c>
       <c r="B18">
-        <v>0.1088083</v>
+        <v>0.2086168</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>42953</v>
+        <v>43234</v>
       </c>
       <c r="B19">
-        <v>0.127551</v>
+        <v>0.1458333</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>42954</v>
+        <v>43265</v>
       </c>
       <c r="B20">
-        <v>0.107438</v>
+        <v>0.1434109</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>42955</v>
+        <v>42922</v>
       </c>
       <c r="B21">
-        <v>0.09157510000000001</v>
+        <v>0.1253644</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>42957</v>
+        <v>42923</v>
       </c>
       <c r="B22">
-        <v>0.1348315</v>
+        <v>0.1050955</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>42966</v>
+        <v>42924</v>
       </c>
       <c r="B23">
-        <v>0.1318052</v>
+        <v>0.1209302</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>42974</v>
+        <v>42930</v>
       </c>
       <c r="B24">
-        <v>0.1198157</v>
+        <v>0.1464435</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>42975</v>
+        <v>42940</v>
       </c>
       <c r="B25">
-        <v>0.1486811</v>
+        <v>0.0988024</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>42979</v>
+        <v>42946</v>
       </c>
       <c r="B26">
-        <v>0.1176471</v>
+        <v>0.1030303</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>42980</v>
+        <v>42947</v>
       </c>
       <c r="B27">
-        <v>0.0943396</v>
+        <v>0.1187905</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>42986</v>
+        <v>42950</v>
       </c>
       <c r="B28">
-        <v>0.07853400000000001</v>
+        <v>0.1437908</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>42989</v>
+        <v>42951</v>
       </c>
       <c r="B29">
-        <v>0.0826446</v>
+        <v>0.1384615</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>42992</v>
+        <v>42952</v>
       </c>
       <c r="B30">
-        <v>0.125</v>
+        <v>0.1088083</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>43000</v>
+        <v>42953</v>
       </c>
       <c r="B31">
-        <v>0.125</v>
+        <v>0.127551</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>43001</v>
+        <v>42954</v>
       </c>
       <c r="B32">
-        <v>0.08119659999999999</v>
+        <v>0.107438</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>43002</v>
+        <v>42955</v>
       </c>
       <c r="B33">
-        <v>0.0841837</v>
+        <v>0.09157510000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>43006</v>
+        <v>42956</v>
       </c>
       <c r="B34">
-        <v>0.07383969999999999</v>
+        <v>0.0634921</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>43007</v>
+        <v>42957</v>
       </c>
       <c r="B35">
-        <v>0.1066282</v>
+        <v>0.1348315</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>43008</v>
+        <v>42966</v>
       </c>
       <c r="B36">
-        <v>0.08053689999999999</v>
+        <v>0.1318052</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>43036</v>
+        <v>42967</v>
       </c>
       <c r="B37">
-        <v>0.1393324</v>
+        <v>0.0808625</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>43037</v>
+        <v>42974</v>
       </c>
       <c r="B38">
-        <v>0.1767372</v>
+        <v>0.1198157</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>43038</v>
+        <v>42975</v>
       </c>
       <c r="B39">
-        <v>0.1458626</v>
+        <v>0.1486811</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>43045</v>
+        <v>42979</v>
       </c>
       <c r="B40">
-        <v>0.3890411</v>
+        <v>0.1176471</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>43048</v>
+        <v>42980</v>
       </c>
       <c r="B41">
-        <v>0.2710997</v>
+        <v>0.0943396</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>43050</v>
+        <v>42986</v>
       </c>
       <c r="B42">
-        <v>0.3011152</v>
+        <v>0.07853400000000001</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>43063</v>
+        <v>42987</v>
       </c>
       <c r="B43">
-        <v>0.3663194</v>
+        <v>0.0524934</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>43095</v>
+        <v>42989</v>
       </c>
       <c r="B44">
-        <v>0.3736264</v>
+        <v>0.0826446</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>43136</v>
+        <v>42991</v>
       </c>
       <c r="B45">
-        <v>0.4263658</v>
+        <v>0.1456693</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>43137</v>
+        <v>42992</v>
       </c>
       <c r="B46">
-        <v>0.4227941</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>43138</v>
+        <v>42994</v>
       </c>
       <c r="B47">
-        <v>0.4769688</v>
+        <v>0.0612245</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>43145</v>
+        <v>43000</v>
       </c>
       <c r="B48">
-        <v>0.6065891</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>43149</v>
+        <v>43001</v>
       </c>
       <c r="B49">
-        <v>0.3625</v>
+        <v>0.08119659999999999</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>43159</v>
+        <v>43002</v>
       </c>
       <c r="B50">
-        <v>0.43898</v>
+        <v>0.0841837</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>43179</v>
+        <v>43006</v>
       </c>
       <c r="B51">
-        <v>0.3502415</v>
+        <v>0.07383969999999999</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>43192</v>
+        <v>43007</v>
       </c>
       <c r="B52">
-        <v>0.4662757</v>
+        <v>0.1066282</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>43206</v>
+        <v>43008</v>
       </c>
       <c r="B53">
-        <v>0.5033408</v>
+        <v>0.08053689999999999</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>43224</v>
+        <v>43010</v>
       </c>
       <c r="B54">
-        <v>0.2011494</v>
+        <v>0.0979782</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>43225</v>
+        <v>43034</v>
       </c>
       <c r="B55">
-        <v>0.1826625</v>
+        <v>0.2241993</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>42924</v>
+        <v>43035</v>
       </c>
       <c r="B56">
-        <v>0.1273585</v>
+        <v>0.213628</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>42925</v>
+        <v>43036</v>
       </c>
       <c r="B57">
-        <v>0.1170213</v>
+        <v>0.1393324</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>42926</v>
+        <v>43037</v>
       </c>
       <c r="B58">
-        <v>0.0847458</v>
+        <v>0.1767372</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>42934</v>
+        <v>43038</v>
       </c>
       <c r="B59">
-        <v>0.0743494</v>
+        <v>0.1458626</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>42937</v>
+        <v>43045</v>
       </c>
       <c r="B60">
-        <v>0.0693069</v>
+        <v>0.3890411</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>42941</v>
+        <v>43048</v>
       </c>
       <c r="B61">
-        <v>0.1190476</v>
+        <v>0.2710997</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>42942</v>
+        <v>43050</v>
       </c>
       <c r="B62">
-        <v>0.0763359</v>
+        <v>0.3011152</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>42949</v>
+        <v>43063</v>
       </c>
       <c r="B63">
-        <v>0.08522730000000001</v>
+        <v>0.3663194</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>42951</v>
+        <v>43070</v>
       </c>
       <c r="B64">
-        <v>0.1472868</v>
+        <v>0.6732026</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>42958</v>
+        <v>43095</v>
       </c>
       <c r="B65">
-        <v>0.1542289</v>
+        <v>0.3736264</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>42959</v>
+        <v>43136</v>
       </c>
       <c r="B66">
-        <v>0.102439</v>
+        <v>0.4263658</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>42966</v>
+        <v>43137</v>
       </c>
       <c r="B67">
-        <v>0.145749</v>
+        <v>0.4227941</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>42970</v>
+        <v>43138</v>
       </c>
       <c r="B68">
-        <v>0.1280488</v>
+        <v>0.4769688</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>42979</v>
+        <v>43145</v>
       </c>
       <c r="B69">
-        <v>0.1192308</v>
+        <v>0.6065891</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>42988</v>
+        <v>43149</v>
       </c>
       <c r="B70">
-        <v>0.1021021</v>
+        <v>0.3625</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>42989</v>
+        <v>43159</v>
       </c>
       <c r="B71">
-        <v>0.0751445</v>
+        <v>0.43898</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>42992</v>
+        <v>43163</v>
       </c>
       <c r="B72">
-        <v>0.09230770000000001</v>
+        <v>0.7392924</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>43001</v>
+        <v>43171</v>
       </c>
       <c r="B73">
-        <v>0.08883249999999999</v>
+        <v>0.6770073</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>43008</v>
+        <v>43172</v>
       </c>
       <c r="B74">
-        <v>0.09090910000000001</v>
+        <v>0.2757732</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>43073</v>
+        <v>43179</v>
       </c>
       <c r="B75">
-        <v>0.5288462</v>
+        <v>0.3502415</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>43090</v>
+        <v>43183</v>
       </c>
       <c r="B76">
-        <v>0.5082873</v>
+        <v>0.2880658</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>43104</v>
+        <v>43192</v>
       </c>
       <c r="B77">
-        <v>0.4344392</v>
+        <v>0.4662757</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>43166</v>
+        <v>43197</v>
       </c>
       <c r="B78">
-        <v>0.6469003</v>
+        <v>0.5641026</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>43175</v>
+        <v>43198</v>
       </c>
       <c r="B79">
-        <v>0.403397</v>
+        <v>0.2566735</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
+        <v>43206</v>
+      </c>
+      <c r="B80">
+        <v>0.5033408</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="2">
+        <v>43223</v>
+      </c>
+      <c r="B81">
+        <v>0.1147059</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2">
+        <v>43224</v>
+      </c>
+      <c r="B82">
+        <v>0.2011494</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2">
+        <v>43225</v>
+      </c>
+      <c r="B83">
+        <v>0.1826625</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2">
+        <v>43226</v>
+      </c>
+      <c r="B84">
+        <v>0.1168478</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="2">
+        <v>43233</v>
+      </c>
+      <c r="B85">
+        <v>0.1375661</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="2">
+        <v>43234</v>
+      </c>
+      <c r="B86">
+        <v>0.1015228</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="2">
+        <v>42924</v>
+      </c>
+      <c r="B87">
+        <v>0.1273585</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="2">
+        <v>42925</v>
+      </c>
+      <c r="B88">
+        <v>0.1170213</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="2">
+        <v>42926</v>
+      </c>
+      <c r="B89">
+        <v>0.0847458</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="2">
+        <v>42927</v>
+      </c>
+      <c r="B90">
+        <v>0.0541516</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="2">
+        <v>42934</v>
+      </c>
+      <c r="B91">
+        <v>0.0743494</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="2">
+        <v>42935</v>
+      </c>
+      <c r="B92">
+        <v>0.0552326</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="2">
+        <v>42936</v>
+      </c>
+      <c r="B93">
+        <v>0.0676157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="2">
+        <v>42937</v>
+      </c>
+      <c r="B94">
+        <v>0.0693069</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="2">
+        <v>42940</v>
+      </c>
+      <c r="B95">
+        <v>0.0637255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="2">
+        <v>42941</v>
+      </c>
+      <c r="B96">
+        <v>0.1190476</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="2">
+        <v>42942</v>
+      </c>
+      <c r="B97">
+        <v>0.0763359</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="2">
+        <v>42949</v>
+      </c>
+      <c r="B98">
+        <v>0.08522730000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="2">
+        <v>42951</v>
+      </c>
+      <c r="B99">
+        <v>0.1472868</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="2">
+        <v>42958</v>
+      </c>
+      <c r="B100">
+        <v>0.1542289</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="2">
+        <v>42959</v>
+      </c>
+      <c r="B101">
+        <v>0.102439</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="2">
+        <v>42961</v>
+      </c>
+      <c r="B102">
+        <v>0.0814815</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2">
+        <v>42962</v>
+      </c>
+      <c r="B103">
+        <v>0.0674157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2">
+        <v>42966</v>
+      </c>
+      <c r="B104">
+        <v>0.145749</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="2">
+        <v>42970</v>
+      </c>
+      <c r="B105">
+        <v>0.1280488</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="2">
+        <v>42971</v>
+      </c>
+      <c r="B106">
+        <v>0.0606061</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="2">
+        <v>42979</v>
+      </c>
+      <c r="B107">
+        <v>0.1192308</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="2">
+        <v>42981</v>
+      </c>
+      <c r="B108">
+        <v>0.06530610000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="2">
+        <v>42988</v>
+      </c>
+      <c r="B109">
+        <v>0.1021021</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="2">
+        <v>42989</v>
+      </c>
+      <c r="B110">
+        <v>0.0751445</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="2">
+        <v>42991</v>
+      </c>
+      <c r="B111">
+        <v>0.1428571</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="2">
+        <v>42992</v>
+      </c>
+      <c r="B112">
+        <v>0.09230770000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="2">
+        <v>42993</v>
+      </c>
+      <c r="B113">
+        <v>0.059761</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="2">
+        <v>43000</v>
+      </c>
+      <c r="B114">
+        <v>0.1466667</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="2">
+        <v>43001</v>
+      </c>
+      <c r="B115">
+        <v>0.08883249999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="2">
+        <v>43002</v>
+      </c>
+      <c r="B116">
+        <v>0.0544218</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="2">
+        <v>43003</v>
+      </c>
+      <c r="B117">
+        <v>0.1377246</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="2">
+        <v>43008</v>
+      </c>
+      <c r="B118">
+        <v>0.09090910000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="2">
+        <v>43009</v>
+      </c>
+      <c r="B119">
+        <v>0.08860759999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="2">
+        <v>43010</v>
+      </c>
+      <c r="B120">
+        <v>0.0822368</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="2">
+        <v>43011</v>
+      </c>
+      <c r="B121">
+        <v>0.0763359</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="2">
+        <v>43016</v>
+      </c>
+      <c r="B122">
+        <v>0.0821678</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="2">
+        <v>43021</v>
+      </c>
+      <c r="B123">
+        <v>0.2177122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="2">
+        <v>43061</v>
+      </c>
+      <c r="B124">
+        <v>0.4081633</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="2">
+        <v>43073</v>
+      </c>
+      <c r="B125">
+        <v>0.5288462</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="2">
+        <v>43087</v>
+      </c>
+      <c r="B126">
+        <v>0.7295775</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="2">
+        <v>43090</v>
+      </c>
+      <c r="B127">
+        <v>0.5082873</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="2">
+        <v>43104</v>
+      </c>
+      <c r="B128">
+        <v>0.4344392</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="2">
+        <v>43152</v>
+      </c>
+      <c r="B129">
+        <v>0.7485822</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="2">
+        <v>43166</v>
+      </c>
+      <c r="B130">
+        <v>0.6469003</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="2">
+        <v>43175</v>
+      </c>
+      <c r="B131">
+        <v>0.403397</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="2">
+        <v>43188</v>
+      </c>
+      <c r="B132">
+        <v>0.2966752</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="2">
+        <v>43197</v>
+      </c>
+      <c r="B133">
+        <v>0.5927602</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="2">
+        <v>43198</v>
+      </c>
+      <c r="B134">
+        <v>0.2231076</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="2">
         <v>43201</v>
       </c>
-      <c r="B80">
+      <c r="B135">
         <v>0.2928571</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="2">
+        <v>43205</v>
+      </c>
+      <c r="B136">
+        <v>0.5315315</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="2">
+        <v>43210</v>
+      </c>
+      <c r="B137">
+        <v>0.3888889</v>
       </c>
     </row>
   </sheetData>
@@ -1841,7 +2809,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1857,137 +2825,201 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>42987</v>
+        <v>43115</v>
       </c>
       <c r="B2">
-        <v>0.1138015</v>
+        <v>0.6528777</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>42990</v>
+        <v>42987</v>
       </c>
       <c r="B3">
-        <v>0.1170213</v>
+        <v>0.1138015</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>42994</v>
+        <v>42990</v>
       </c>
       <c r="B4">
-        <v>0.1119792</v>
+        <v>0.1170213</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>42995</v>
+        <v>42992</v>
       </c>
       <c r="B5">
-        <v>0.114094</v>
+        <v>0.1428571</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>42996</v>
+        <v>42994</v>
       </c>
       <c r="B6">
-        <v>0.1305263</v>
+        <v>0.1119792</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>43002</v>
+        <v>42995</v>
       </c>
       <c r="B7">
-        <v>0.1041667</v>
+        <v>0.114094</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>43006</v>
+        <v>42996</v>
       </c>
       <c r="B8">
-        <v>0.0888383</v>
+        <v>0.1305263</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>43010</v>
+        <v>43002</v>
       </c>
       <c r="B9">
-        <v>0.1278863</v>
+        <v>0.1041667</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>43019</v>
+        <v>43006</v>
       </c>
       <c r="B10">
-        <v>0.1828442</v>
+        <v>0.0888383</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>43020</v>
+        <v>43007</v>
       </c>
       <c r="B11">
-        <v>0.1438053</v>
+        <v>0.1384615</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>43021</v>
+        <v>43009</v>
       </c>
       <c r="B12">
-        <v>0.1268382</v>
+        <v>0.0887681</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>43035</v>
+        <v>43010</v>
       </c>
       <c r="B13">
-        <v>0.1889764</v>
+        <v>0.1278863</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>43043</v>
+        <v>43018</v>
       </c>
       <c r="B14">
-        <v>0.3365617</v>
+        <v>0.1966019</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>43083</v>
+        <v>43019</v>
       </c>
       <c r="B15">
-        <v>0.5813952999999999</v>
+        <v>0.1828442</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>43127</v>
+        <v>43020</v>
       </c>
       <c r="B16">
-        <v>0.3636364</v>
+        <v>0.1438053</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>43133</v>
+        <v>43021</v>
       </c>
       <c r="B17">
-        <v>0.3642241</v>
+        <v>0.1268382</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
+        <v>43035</v>
+      </c>
+      <c r="B18">
+        <v>0.1889764</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2">
+        <v>43040</v>
+      </c>
+      <c r="B19">
+        <v>0.4084778</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2">
+        <v>43043</v>
+      </c>
+      <c r="B20">
+        <v>0.3365617</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2">
+        <v>43083</v>
+      </c>
+      <c r="B21">
+        <v>0.5813952999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2">
+        <v>43127</v>
+      </c>
+      <c r="B22">
+        <v>0.3636364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2">
+        <v>43128</v>
+      </c>
+      <c r="B23">
+        <v>0.3379416</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2">
+        <v>43132</v>
+      </c>
+      <c r="B24">
+        <v>0.2920792</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2">
+        <v>43133</v>
+      </c>
+      <c r="B25">
+        <v>0.3642241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2">
         <v>43134</v>
       </c>
-      <c r="B18">
+      <c r="B26">
         <v>0.5736926</v>
       </c>
     </row>
@@ -1998,7 +3030,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2022,217 +3054,313 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>43130</v>
+        <v>43129</v>
       </c>
       <c r="B3">
-        <v>0.535316</v>
+        <v>0.3320826</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>42987</v>
+        <v>43130</v>
       </c>
       <c r="B4">
-        <v>0.1138015</v>
+        <v>0.535316</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>42995</v>
+        <v>42987</v>
       </c>
       <c r="B5">
-        <v>0.09843399999999999</v>
+        <v>0.1138015</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>42998</v>
+        <v>42993</v>
       </c>
       <c r="B6">
-        <v>0.1011673</v>
+        <v>0.1356784</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>43007</v>
+        <v>42995</v>
       </c>
       <c r="B7">
-        <v>0.08461539999999999</v>
+        <v>0.09843399999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>43010</v>
+        <v>42996</v>
       </c>
       <c r="B8">
-        <v>0.1332149</v>
+        <v>0.1389474</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>43020</v>
+        <v>42998</v>
       </c>
       <c r="B9">
-        <v>0.1637168</v>
+        <v>0.1011673</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>43021</v>
+        <v>43007</v>
       </c>
       <c r="B10">
-        <v>0.1709559</v>
+        <v>0.08461539999999999</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>43053</v>
+        <v>43010</v>
       </c>
       <c r="B11">
-        <v>0.2340426</v>
+        <v>0.1332149</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>43062</v>
+        <v>43018</v>
       </c>
       <c r="B12">
-        <v>0.3317647</v>
+        <v>0.2135922</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>43067</v>
+        <v>43019</v>
       </c>
       <c r="B13">
-        <v>0.223565</v>
+        <v>0.2189616</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>43073</v>
+        <v>43020</v>
       </c>
       <c r="B14">
-        <v>0.315197</v>
+        <v>0.1637168</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>43074</v>
+        <v>43021</v>
       </c>
       <c r="B15">
-        <v>0.2943662</v>
+        <v>0.1709559</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>43088</v>
+        <v>43034</v>
       </c>
       <c r="B16">
-        <v>0.2971429</v>
+        <v>0.2209738</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>43093</v>
+        <v>43053</v>
       </c>
       <c r="B17">
-        <v>0.3267717</v>
+        <v>0.2340426</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>43096</v>
+        <v>43062</v>
       </c>
       <c r="B18">
-        <v>0.3533026</v>
+        <v>0.3317647</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>43098</v>
+        <v>43067</v>
       </c>
       <c r="B19">
-        <v>0.3410138</v>
+        <v>0.223565</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>43099</v>
+        <v>43070</v>
       </c>
       <c r="B20">
-        <v>0.2560241</v>
+        <v>0.2972973</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>43114</v>
+        <v>43073</v>
       </c>
       <c r="B21">
-        <v>0.3317972</v>
+        <v>0.315197</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>43126</v>
+        <v>43074</v>
       </c>
       <c r="B22">
-        <v>0.5483871</v>
+        <v>0.2943662</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>43127</v>
+        <v>43088</v>
       </c>
       <c r="B23">
-        <v>0.3723776</v>
+        <v>0.2971429</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>43132</v>
+        <v>43093</v>
       </c>
       <c r="B24">
-        <v>0.3333333</v>
+        <v>0.3267717</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>43134</v>
+        <v>43095</v>
       </c>
       <c r="B25">
-        <v>0.3359746</v>
+        <v>0.4008942</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>42968</v>
+        <v>43096</v>
       </c>
       <c r="B26">
-        <v>0.1502347</v>
+        <v>0.3533026</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>42971</v>
+        <v>43098</v>
       </c>
       <c r="B27">
-        <v>0.095679</v>
+        <v>0.3410138</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>43021</v>
+        <v>43099</v>
       </c>
       <c r="B28">
-        <v>0.1943888</v>
+        <v>0.2560241</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
+        <v>43114</v>
+      </c>
+      <c r="B29">
+        <v>0.3317972</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2">
+        <v>43120</v>
+      </c>
+      <c r="B30">
+        <v>0.7443609</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2">
+        <v>43125</v>
+      </c>
+      <c r="B31">
+        <v>0.7441077</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
+        <v>43126</v>
+      </c>
+      <c r="B32">
+        <v>0.5483871</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
+        <v>43127</v>
+      </c>
+      <c r="B33">
+        <v>0.3723776</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2">
+        <v>43128</v>
+      </c>
+      <c r="B34">
+        <v>0.3010753</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2">
+        <v>43132</v>
+      </c>
+      <c r="B35">
+        <v>0.3333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2">
+        <v>43134</v>
+      </c>
+      <c r="B36">
+        <v>0.3359746</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2">
+        <v>42935</v>
+      </c>
+      <c r="B37">
+        <v>0.1382488</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2">
+        <v>42968</v>
+      </c>
+      <c r="B38">
+        <v>0.1502347</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2">
+        <v>42971</v>
+      </c>
+      <c r="B39">
+        <v>0.095679</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2">
+        <v>43021</v>
+      </c>
+      <c r="B40">
+        <v>0.1943888</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2">
         <v>43121</v>
       </c>
-      <c r="B29">
+      <c r="B41">
         <v>0.3660856</v>
       </c>
     </row>
@@ -2243,7 +3371,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2259,594 +3387,594 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>43114</v>
+        <v>43106</v>
       </c>
       <c r="B2">
-        <v>0.451664</v>
+        <v>0.2743506</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>43116</v>
+        <v>43111</v>
       </c>
       <c r="B3">
-        <v>0.5191041</v>
+        <v>0.3188623</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>43118</v>
+        <v>43114</v>
       </c>
       <c r="B4">
-        <v>0.6185853</v>
+        <v>0.451664</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>43123</v>
+        <v>43116</v>
       </c>
       <c r="B5">
-        <v>0.4397993</v>
+        <v>0.5191041</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>43131</v>
+        <v>43118</v>
       </c>
       <c r="B6">
-        <v>0.3900344</v>
+        <v>0.6185853</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>43146</v>
+        <v>43123</v>
       </c>
       <c r="B7">
-        <v>0.6424051</v>
+        <v>0.4397993</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>43147</v>
+        <v>43131</v>
       </c>
       <c r="B8">
-        <v>0.3713235</v>
+        <v>0.3900344</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>43151</v>
+        <v>43146</v>
       </c>
       <c r="B9">
-        <v>0.5538695</v>
+        <v>0.6424051</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>43152</v>
+        <v>43147</v>
       </c>
       <c r="B10">
-        <v>0.4393305</v>
+        <v>0.3713235</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>43158</v>
+        <v>43151</v>
       </c>
       <c r="B11">
-        <v>0.4030303</v>
+        <v>0.5538695</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>43180</v>
+        <v>43152</v>
       </c>
       <c r="B12">
-        <v>0.4752137</v>
+        <v>0.4393305</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>43201</v>
+        <v>43154</v>
       </c>
       <c r="B13">
-        <v>0.2924791</v>
+        <v>0.2943038</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>43205</v>
+        <v>43158</v>
       </c>
       <c r="B14">
-        <v>0.2696897</v>
+        <v>0.4030303</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>43215</v>
+        <v>43180</v>
       </c>
       <c r="B15">
-        <v>0.35</v>
+        <v>0.4752137</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>43228</v>
+        <v>43188</v>
       </c>
       <c r="B16">
-        <v>0.2068966</v>
+        <v>0.2478992</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>43232</v>
+        <v>43196</v>
       </c>
       <c r="B17">
-        <v>0.2135417</v>
+        <v>0.5952891</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>43265</v>
+        <v>43201</v>
       </c>
       <c r="B18">
-        <v>0.1046512</v>
+        <v>0.2924791</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>42922</v>
+        <v>43205</v>
       </c>
       <c r="B19">
-        <v>0.122449</v>
+        <v>0.2696897</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>42923</v>
+        <v>43210</v>
       </c>
       <c r="B20">
-        <v>0.1146497</v>
+        <v>0.5496368</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>42940</v>
+        <v>43213</v>
       </c>
       <c r="B21">
-        <v>0.1107784</v>
+        <v>0.2200436</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>42947</v>
+        <v>43215</v>
       </c>
       <c r="B22">
-        <v>0.0993521</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>42952</v>
+        <v>43228</v>
       </c>
       <c r="B23">
-        <v>0.1243523</v>
+        <v>0.2068966</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>42954</v>
+        <v>43232</v>
       </c>
       <c r="B24">
-        <v>0.1487603</v>
+        <v>0.2135417</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>42955</v>
+        <v>43265</v>
       </c>
       <c r="B25">
-        <v>0.1172161</v>
+        <v>0.1046512</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>42979</v>
+        <v>42921</v>
       </c>
       <c r="B26">
-        <v>0.1232493</v>
+        <v>0.1371951</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>42980</v>
+        <v>42922</v>
       </c>
       <c r="B27">
-        <v>0.0825472</v>
+        <v>0.122449</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>42981</v>
+        <v>42923</v>
       </c>
       <c r="B28">
-        <v>0.07142859999999999</v>
+        <v>0.1146497</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>42993</v>
+        <v>42940</v>
       </c>
       <c r="B29">
-        <v>0.0786517</v>
+        <v>0.1107784</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>42994</v>
+        <v>42947</v>
       </c>
       <c r="B30">
-        <v>0.0932945</v>
+        <v>0.0993521</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>42997</v>
+        <v>42952</v>
       </c>
       <c r="B31">
-        <v>0.08398949999999999</v>
+        <v>0.1243523</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>43000</v>
+        <v>42954</v>
       </c>
       <c r="B32">
-        <v>0.094697</v>
+        <v>0.1487603</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>43001</v>
+        <v>42955</v>
       </c>
       <c r="B33">
-        <v>0.0705128</v>
+        <v>0.1172161</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>43002</v>
+        <v>42957</v>
       </c>
       <c r="B34">
-        <v>0.0841837</v>
+        <v>0.1573034</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>43007</v>
+        <v>42967</v>
       </c>
       <c r="B35">
-        <v>0.0835735</v>
+        <v>0.1698113</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>43018</v>
+        <v>42975</v>
       </c>
       <c r="B36">
-        <v>0.1855422</v>
+        <v>0.17506</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>43036</v>
+        <v>42979</v>
       </c>
       <c r="B37">
-        <v>0.1872279</v>
+        <v>0.1232493</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>43040</v>
+        <v>42980</v>
       </c>
       <c r="B38">
-        <v>0.2715827</v>
+        <v>0.0825472</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>43066</v>
+        <v>42981</v>
       </c>
       <c r="B39">
-        <v>0.2176235</v>
+        <v>0.07142859999999999</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>43088</v>
+        <v>42982</v>
       </c>
       <c r="B40">
-        <v>0.4149933</v>
+        <v>0.0533333</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>43096</v>
+        <v>42988</v>
       </c>
       <c r="B41">
-        <v>0.3839662</v>
+        <v>0.0507614</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>43104</v>
+        <v>42989</v>
       </c>
       <c r="B42">
-        <v>0.5576923</v>
+        <v>0.1404959</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>43137</v>
+        <v>42990</v>
       </c>
       <c r="B43">
-        <v>0.5514706</v>
+        <v>0.0668449</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>43149</v>
+        <v>42992</v>
       </c>
       <c r="B44">
-        <v>0.4791667</v>
+        <v>0.1418919</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>43164</v>
+        <v>42993</v>
       </c>
       <c r="B45">
-        <v>0.3944954</v>
+        <v>0.0786517</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>43172</v>
+        <v>42994</v>
       </c>
       <c r="B46">
-        <v>0.2525773</v>
+        <v>0.0932945</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>43183</v>
+        <v>42997</v>
       </c>
       <c r="B47">
-        <v>0.2880658</v>
+        <v>0.08398949999999999</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>43189</v>
+        <v>42998</v>
       </c>
       <c r="B48">
-        <v>0.3628692</v>
+        <v>0.0522523</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>43193</v>
+        <v>42999</v>
       </c>
       <c r="B49">
-        <v>0.3198198</v>
+        <v>0.0539084</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>43226</v>
+        <v>43000</v>
       </c>
       <c r="B50">
-        <v>0.1657609</v>
+        <v>0.094697</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>43261</v>
+        <v>43001</v>
       </c>
       <c r="B51">
-        <v>0.0943396</v>
+        <v>0.0705128</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>42935</v>
+        <v>43002</v>
       </c>
       <c r="B52">
-        <v>0.1046512</v>
+        <v>0.0841837</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>42936</v>
+        <v>43006</v>
       </c>
       <c r="B53">
-        <v>0.1209964</v>
+        <v>0.0590717</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>42937</v>
+        <v>43007</v>
       </c>
       <c r="B54">
-        <v>0.0990099</v>
+        <v>0.0835735</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>42939</v>
+        <v>43008</v>
       </c>
       <c r="B55">
-        <v>0.0695187</v>
+        <v>0.064877</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>42940</v>
+        <v>43010</v>
       </c>
       <c r="B56">
-        <v>0.1127451</v>
+        <v>0.0917574</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>42942</v>
+        <v>43017</v>
       </c>
       <c r="B57">
-        <v>0.0839695</v>
+        <v>0.2189189</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>42949</v>
+        <v>43018</v>
       </c>
       <c r="B58">
-        <v>0.1420455</v>
+        <v>0.1855422</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>42950</v>
+        <v>43020</v>
       </c>
       <c r="B59">
-        <v>0.09230770000000001</v>
+        <v>0.1954545</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>42951</v>
+        <v>43021</v>
       </c>
       <c r="B60">
-        <v>0.124031</v>
+        <v>0.2073955</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>42961</v>
+        <v>43036</v>
       </c>
       <c r="B61">
-        <v>0.1259259</v>
+        <v>0.1872279</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>42970</v>
+        <v>43040</v>
       </c>
       <c r="B62">
-        <v>0.1158537</v>
+        <v>0.2715827</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>42971</v>
+        <v>43066</v>
       </c>
       <c r="B63">
-        <v>0.1022727</v>
+        <v>0.2176235</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>42993</v>
+        <v>43075</v>
       </c>
       <c r="B64">
-        <v>0.1155378</v>
+        <v>0.6756757</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>43012</v>
+        <v>43078</v>
       </c>
       <c r="B65">
-        <v>0.1945525</v>
+        <v>0.3295292</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>43013</v>
+        <v>43088</v>
       </c>
       <c r="B66">
-        <v>0.1259542</v>
+        <v>0.4149933</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>43014</v>
+        <v>43095</v>
       </c>
       <c r="B67">
-        <v>0.1254545</v>
+        <v>0.7197802</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>43015</v>
+        <v>43096</v>
       </c>
       <c r="B68">
-        <v>0.1403813</v>
+        <v>0.3839662</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>43042</v>
+        <v>43104</v>
       </c>
       <c r="B69">
-        <v>0.3282548</v>
+        <v>0.5576923</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>43073</v>
+        <v>43137</v>
       </c>
       <c r="B70">
-        <v>0.4278075</v>
+        <v>0.5514706</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>43109</v>
+        <v>43146</v>
       </c>
       <c r="B71">
-        <v>0.4695122</v>
+        <v>0.3402923</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>43137</v>
+        <v>43149</v>
       </c>
       <c r="B72">
-        <v>0.5022971000000001</v>
+        <v>0.4791667</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>43176</v>
+        <v>43164</v>
       </c>
       <c r="B73">
-        <v>0.4233871</v>
+        <v>0.3944954</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>43177</v>
+        <v>43172</v>
       </c>
       <c r="B74">
-        <v>0.4324324</v>
+        <v>0.2525773</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>43178</v>
+        <v>43183</v>
       </c>
       <c r="B75">
-        <v>0.3315927</v>
+        <v>0.2880658</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2854,7 +3982,375 @@
         <v>43189</v>
       </c>
       <c r="B76">
+        <v>0.3628692</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="2">
+        <v>43193</v>
+      </c>
+      <c r="B77">
+        <v>0.3198198</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="2">
+        <v>43223</v>
+      </c>
+      <c r="B78">
+        <v>0.2823529</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="2">
+        <v>43226</v>
+      </c>
+      <c r="B79">
+        <v>0.1657609</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="2">
+        <v>43234</v>
+      </c>
+      <c r="B80">
+        <v>0.2436548</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="2">
+        <v>43235</v>
+      </c>
+      <c r="B81">
+        <v>0.1153846</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2">
+        <v>43261</v>
+      </c>
+      <c r="B82">
+        <v>0.0943396</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2">
+        <v>42934</v>
+      </c>
+      <c r="B83">
+        <v>0.133829</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2">
+        <v>42935</v>
+      </c>
+      <c r="B84">
+        <v>0.1046512</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="2">
+        <v>42936</v>
+      </c>
+      <c r="B85">
+        <v>0.1209964</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="2">
+        <v>42937</v>
+      </c>
+      <c r="B86">
+        <v>0.0990099</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="2">
+        <v>42938</v>
+      </c>
+      <c r="B87">
+        <v>0.0676692</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="2">
+        <v>42939</v>
+      </c>
+      <c r="B88">
+        <v>0.0695187</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="2">
+        <v>42940</v>
+      </c>
+      <c r="B89">
+        <v>0.1127451</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="2">
+        <v>42941</v>
+      </c>
+      <c r="B90">
+        <v>0.1428571</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="2">
+        <v>42942</v>
+      </c>
+      <c r="B91">
+        <v>0.0839695</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="2">
+        <v>42949</v>
+      </c>
+      <c r="B92">
+        <v>0.1420455</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="2">
+        <v>42950</v>
+      </c>
+      <c r="B93">
+        <v>0.09230770000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="2">
+        <v>42951</v>
+      </c>
+      <c r="B94">
+        <v>0.124031</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="2">
+        <v>42961</v>
+      </c>
+      <c r="B95">
+        <v>0.1259259</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="2">
+        <v>42962</v>
+      </c>
+      <c r="B96">
+        <v>0.1741573</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="2">
+        <v>42966</v>
+      </c>
+      <c r="B97">
+        <v>0.1619433</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="2">
+        <v>42970</v>
+      </c>
+      <c r="B98">
+        <v>0.1158537</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="2">
+        <v>42971</v>
+      </c>
+      <c r="B99">
+        <v>0.1022727</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="2">
+        <v>42989</v>
+      </c>
+      <c r="B100">
+        <v>0.1416185</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="2">
+        <v>42992</v>
+      </c>
+      <c r="B101">
+        <v>0.1435897</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="2">
+        <v>42993</v>
+      </c>
+      <c r="B102">
+        <v>0.1155378</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2">
+        <v>43009</v>
+      </c>
+      <c r="B103">
+        <v>0.2126582</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2">
+        <v>43012</v>
+      </c>
+      <c r="B104">
+        <v>0.1945525</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="2">
+        <v>43013</v>
+      </c>
+      <c r="B105">
+        <v>0.1259542</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="2">
+        <v>43014</v>
+      </c>
+      <c r="B106">
+        <v>0.1254545</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="2">
+        <v>43015</v>
+      </c>
+      <c r="B107">
+        <v>0.1403813</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="2">
+        <v>43042</v>
+      </c>
+      <c r="B108">
+        <v>0.3282548</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="2">
+        <v>43073</v>
+      </c>
+      <c r="B109">
+        <v>0.4278075</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="2">
+        <v>43090</v>
+      </c>
+      <c r="B110">
+        <v>0.6850829000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="2">
+        <v>43109</v>
+      </c>
+      <c r="B111">
+        <v>0.4695122</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="2">
+        <v>43136</v>
+      </c>
+      <c r="B112">
+        <v>0.7030995</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="2">
+        <v>43137</v>
+      </c>
+      <c r="B113">
+        <v>0.5022971000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="2">
+        <v>43140</v>
+      </c>
+      <c r="B114">
+        <v>0.7040998000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="2">
+        <v>43176</v>
+      </c>
+      <c r="B115">
+        <v>0.4233871</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="2">
+        <v>43177</v>
+      </c>
+      <c r="B116">
+        <v>0.4324324</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="2">
+        <v>43178</v>
+      </c>
+      <c r="B117">
+        <v>0.3315927</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="2">
+        <v>43179</v>
+      </c>
+      <c r="B118">
+        <v>0.2491909</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="2">
+        <v>43189</v>
+      </c>
+      <c r="B119">
         <v>0.4217252</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="2">
+        <v>43190</v>
+      </c>
+      <c r="B120">
+        <v>0.204</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="2">
+        <v>43212</v>
+      </c>
+      <c r="B121">
+        <v>0.5516432</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="2">
+        <v>43213</v>
+      </c>
+      <c r="B122">
+        <v>0.414966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>